<commit_message>
Update baru, menambahkan fitur diskusi (belum sempurna)
</commit_message>
<xml_diff>
--- a/app/Scriptpy/Data Prediksi Tanam.xlsx
+++ b/app/Scriptpy/Data Prediksi Tanam.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViCtus\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laragon\www\PPL\app\Scriptpy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C8186F-8D8C-4380-B377-11BFCF0BC08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF78A45-002F-4254-B413-D2228D169DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{63999A70-0B88-473B-9DE4-36CBBA26F11B}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{63999A70-0B88-473B-9DE4-36CBBA26F11B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -503,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCFC2361-309C-4824-983B-0E0C70EDB8A6}">
   <dimension ref="A1:J1153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1127" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A1141" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1155" sqref="C1155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>